<commit_message>
parser fetch total time info
</commit_message>
<xml_diff>
--- a/pycuda_dev/final_results/results_schedule.xlsx
+++ b/pycuda_dev/final_results/results_schedule.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
-  <si>
-    <t xml:space="preserve">if there’s an X, then we ran it!</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+  <si>
+    <t xml:space="preserve">if there’s a node id, then we ran it!</t>
   </si>
   <si>
     <t xml:space="preserve">CPU</t>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">4-1-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t02n41</t>
   </si>
   <si>
     <t xml:space="preserve">128x16x16</t>
@@ -142,7 +145,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -156,6 +159,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -179,7 +186,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -234,54 +241,84 @@
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="C5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>10</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
up-to-date worksheet with tests
</commit_message>
<xml_diff>
--- a/pycuda_dev/final_results/results_schedule.xlsx
+++ b/pycuda_dev/final_results/results_schedule.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t xml:space="preserve">if there’s a node id, then we started running it!</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">t02n41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t03n06</t>
   </si>
   <si>
     <t xml:space="preserve">128x16x16</t>
@@ -93,7 +96,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -114,6 +117,29 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF00CC00"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -158,7 +184,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -171,7 +197,43 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -188,6 +250,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00CC00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -196,177 +318,302 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1683673469388"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.1173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.16326530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="3.12244897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.1173469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.16326530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="1.72959183673469"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="2.16836734693878"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="1.81632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0"/>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="0"/>
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0"/>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="C2" s="0"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0"/>
+      <c r="C3" s="0"/>
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E4" s="5"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="H4" s="5"/>
+      <c r="J4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="K4" s="7"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0"/>
+      <c r="N4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="B5" s="0"/>
+      <c r="C5" s="0"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="6"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="13" t="n">
+        <v>182</v>
+      </c>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="13" t="n">
+        <v>182</v>
+      </c>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="B8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="B9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="F11" s="12"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:G2"/>
+  <mergeCells count="7">
+    <mergeCell ref="D1:N1"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="M4:N4"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>